<commit_message>
modified to able to operate on multiple arbitrage analysis
</commit_message>
<xml_diff>
--- a/Stocks.xlsx
+++ b/Stocks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaelxu/My_Document/Michael/金融/量化/Arbitrage/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E6D856E-CBED-8A46-BEE0-E2CE84A68AB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{512F832F-CC64-5F4D-8E5A-A1B6B1730D17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15360" yWindow="500" windowWidth="15360" windowHeight="17720" activeTab="1" xr2:uid="{49E41F07-E01F-DB49-9AD6-EC869743E72B}"/>
+    <workbookView xWindow="40" yWindow="500" windowWidth="18860" windowHeight="17720" activeTab="1" xr2:uid="{49E41F07-E01F-DB49-9AD6-EC869743E72B}"/>
   </bookViews>
   <sheets>
     <sheet name="Watchlist" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="742" uniqueCount="426">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="752" uniqueCount="436">
   <si>
     <t>603993.SS</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1353,10 +1353,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>‘601857.SS', '600028.SS', '600256.SS', '601139.SS', '600777.SS', '600759.SS', '605368.SS', '600617.SS', '002700.SZ', '000669.SZ', '000968.SZ'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>601088.SS', '600989.SS', '600803.SS', '600256.SS', '600546.SS',  '600121.SS', '600397.SS', '600740.SS', '000983.SZ', '600792.SS', '601225.SS', '601001.SS', '600403.SS'</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1378,6 +1374,49 @@
   </si>
   <si>
     <t>000422.SZ', '000603.SZ', '605086.SS', '600459.SS', '603132.SS', '000960.SZ', '600490.SS'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>300750.SZ', '300014.SZ', '002466.SZ', '002466.SZ', '002340.SZ', '300207.SZ', '300919.SZ', '688772.SS', '002407.SZ', '301219.SZ', '002240.SZ', '002497.SZ', '300438.SZ', '000049.SZ'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>300014.SZ', '002460.SZ', '301219.SZ', '002240.SZ', '002192.SZ', '300890.SZ'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>601168.SS', '000933.SZ', '601212.SS', '000060.SZ', '002182.SZ', '600595.SS', '000612.SZ', '600531.SS', '002578.SZ', '1378.HK'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>003816.SZ', '600023.SS', '601991.SS', '000027.SZ', '000690.SZ', '000791.SZ', '600900.SS'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>600848.SS', '600736.SS', '600748.SS', '600340.SS', '600658.SS', '600638.SS'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>003816.SZ', '600025.SS', '600886.SS', '600795.SS', '600236.SS', '600310.SS', '000993.SZ'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>600018.SS', '000039.SZ', '601000.SS', '603565.SS', '601022.SS', '600179.SS', '000520.SZ', '1308.HK', '0716.HK', '1919.HK', '603162.SS', '603209.SS', '601872.SS', '600428.SS', '601975.SS', '601919.SS', '601866.SS', '001205.SZ', '601022.SS', '600798.SS', '601083.SS', '1138.HK'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>603993.SS, 002460.SZ, 603799.SS, 002340.SZ, 002709.SZ, 300919.SZ, 603659.SS, 600884.SS, 600711.SS, 301219.SZ, 688005.SS, 300618.SZ, 300409.SZ, 600490.SS, 002741.SZ, 688707.SS, 688275.SS, 301152.SZ, 001283.SZ, 688148.SS, 688184.SS</t>
+  </si>
+  <si>
+    <t>600018.SS, 601298.SS, 001872.SZ, 601000.SS, 601866.SS, 601880.SS, 601228.SS, 000088.SZ, 600320.SS, 600717.SS, 601008.SS, 6198.HK</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>601857.SS', '600028.SS', '600256.SS', '601139.SS', '600777.SS', '600759.SS', '605368.SS', '600617.SS', '002700.SZ', '000669.SZ', '000968.SZ'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>601168.SS, 601020.SS, 000426.SZ, 600490.SS, 000975.SZ, 601212.SS, 002716.SZ, 000603.SZ, 601069.SS, 600988.SS, 600916.SS, 002237.SZ, 000060.SZ, 603132.SS, 600338.SS, 000688.SZ, 600497.SS, 1818.HK, 0661.HK</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1835,7 +1874,7 @@
   <dimension ref="A1:I34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:C21"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1865,7 +1904,7 @@
       </c>
       <c r="E1" s="1">
         <f ca="1">TODAY()</f>
-        <v>45502</v>
+        <v>45503</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>341</v>
@@ -1891,7 +1930,7 @@
       </c>
       <c r="D2" s="2">
         <f ca="1">[1]!s_val_mv_ref(B2,$E$1,100000000)</f>
-        <v>162.51241855999999</v>
+        <v>163.63147882000001</v>
       </c>
       <c r="F2" t="str">
         <f>[1]!s_info_thematicindustry_wind(B2,"")</f>
@@ -1912,7 +1951,7 @@
       </c>
       <c r="D3" s="2">
         <f ca="1">[1]!s_val_mv_ref(B3,$E$1,100000000)</f>
-        <v>14084.51881566</v>
+        <v>13351.990650309999</v>
       </c>
       <c r="F3" t="str">
         <f>[1]!s_info_thematicindustry_wind(B3,"")</f>
@@ -1933,7 +1972,7 @@
       </c>
       <c r="D4" s="2">
         <f ca="1">[1]!s_val_mv_ref(B4,$E$1,100000000)</f>
-        <v>2283.1725000000001</v>
+        <v>2223.0635000000002</v>
       </c>
       <c r="F4" t="str">
         <f>[1]!s_info_thematicindustry_wind(B4,"")</f>
@@ -1960,7 +1999,7 @@
       </c>
       <c r="D5" s="2">
         <f ca="1">[1]!s_val_mv_ref(B5,$E$1,100000000)</f>
-        <v>1591.039608</v>
+        <v>1535.35322172</v>
       </c>
       <c r="F5" t="str">
         <f>[1]!s_info_thematicindustry_wind(B5,"")</f>
@@ -1987,7 +2026,7 @@
       </c>
       <c r="D6" s="2">
         <f ca="1">[1]!s_val_mv_ref(B6,$E$1,100000000)</f>
-        <v>1589.7041069100001</v>
+        <v>1546.5056257399999</v>
       </c>
       <c r="F6" t="str">
         <f>[1]!s_info_thematicindustry_wind(B6,"")</f>
@@ -2014,7 +2053,7 @@
       </c>
       <c r="D7" s="2">
         <f ca="1">[1]!s_val_mv_ref(B7,$E$1,100000000)</f>
-        <v>617.81475239999997</v>
+        <v>619.98379190000003</v>
       </c>
       <c r="F7" t="str">
         <f>[1]!s_info_thematicindustry_wind(B7,"")</f>
@@ -2044,7 +2083,7 @@
       </c>
       <c r="D8" s="2">
         <f ca="1">[1]!s_val_mv_ref(B8,$E$1,100000000)</f>
-        <v>245.35425058000001</v>
+        <v>243.86854145000001</v>
       </c>
       <c r="F8" t="str">
         <f>[1]!s_info_thematicindustry_wind(B8,"")</f>
@@ -2071,7 +2110,7 @@
       </c>
       <c r="D9" s="2">
         <f ca="1">[1]!s_val_mv_ref(B9,$E$1,100000000)</f>
-        <v>541.60954865999997</v>
+        <v>537.97864665999998</v>
       </c>
       <c r="F9" t="str">
         <f>[1]!s_info_thematicindustry_wind(B9,"")</f>
@@ -2092,7 +2131,7 @@
       </c>
       <c r="D10" s="2">
         <f ca="1">[1]!s_val_mv_ref(B10,$E$1,100000000)</f>
-        <v>462.33211992999998</v>
+        <v>461.01914266</v>
       </c>
       <c r="F10" t="str">
         <f>[1]!s_info_thematicindustry_wind(B10,"")</f>
@@ -2113,7 +2152,7 @@
       </c>
       <c r="D11" s="2">
         <f ca="1">[1]!s_val_mv_ref(B11,$E$1,100000000)</f>
-        <v>1173.633276</v>
+        <v>1134.16899917</v>
       </c>
       <c r="F11" t="str">
         <f>[1]!s_info_thematicindustry_wind(B11,"")</f>
@@ -2134,7 +2173,7 @@
       </c>
       <c r="D12" s="2">
         <f ca="1">[1]!s_val_mv_ref(B12,$E$1,100000000)</f>
-        <v>381.53346419000002</v>
+        <v>378.30875965000001</v>
       </c>
       <c r="F12" t="str">
         <f>[1]!s_info_thematicindustry_wind(B12,"")</f>
@@ -2155,7 +2194,7 @@
       </c>
       <c r="D13" s="2">
         <f ca="1">[1]!s_val_mv_ref(B13,$E$1,100000000)</f>
-        <v>2084.4551390299998</v>
+        <v>2058.9181694899999</v>
       </c>
       <c r="F13" t="str">
         <f>[1]!s_info_thematicindustry_wind(B13,"")</f>
@@ -2176,7 +2215,7 @@
       </c>
       <c r="D14" s="2">
         <f ca="1">[1]!s_val_mv_ref(B14,$E$1,100000000)</f>
-        <v>700.34997479000003</v>
+        <v>703.21244062000005</v>
       </c>
       <c r="F14" t="str">
         <f>[1]!s_info_thematicindustry_wind(B14,"")</f>
@@ -2203,7 +2242,7 @@
       </c>
       <c r="D15" s="2">
         <f ca="1">[1]!s_val_mv_ref(B15,$E$1,100000000)</f>
-        <v>472.87580172999998</v>
+        <v>474.81950732000001</v>
       </c>
       <c r="F15" t="str">
         <f>[1]!s_info_thematicindustry_wind(B15,"")</f>
@@ -2224,7 +2263,7 @@
       </c>
       <c r="D16" s="2">
         <f ca="1">[1]!s_val_mv_ref(B16,$E$1,100000000)</f>
-        <v>196.05263821</v>
+        <v>199.29814479000001</v>
       </c>
       <c r="F16" t="str">
         <f>[1]!s_info_thematicindustry_wind(B16,"")</f>
@@ -2251,7 +2290,7 @@
       </c>
       <c r="D17" s="2">
         <f ca="1">[1]!s_val_mv_ref(B17,$E$1,100000000)</f>
-        <v>108.73834964</v>
+        <v>111.07884931</v>
       </c>
       <c r="F17" t="str">
         <f>[1]!s_info_thematicindustry_wind(B17,"")</f>
@@ -2308,7 +2347,7 @@
       </c>
       <c r="D19" s="2">
         <f ca="1">[1]!s_val_mv_ref(B19,$E$1,100000000)</f>
-        <v>287.12704257000001</v>
+        <v>301.37498642999998</v>
       </c>
       <c r="F19" t="str">
         <f>[1]!s_info_thematicindustry_wind(B19,"")</f>
@@ -2335,7 +2374,7 @@
       </c>
       <c r="D20" s="2">
         <f ca="1">[1]!s_val_mv_ref(B20,$E$1,100000000)</f>
-        <v>2247.1108991699998</v>
+        <v>2192.3493730599998</v>
       </c>
       <c r="F20" t="str">
         <f>[1]!s_info_thematicindustry_wind(B20,"")</f>
@@ -2362,7 +2401,7 @@
       </c>
       <c r="D21" s="2">
         <f ca="1">[1]!s_val_mv_ref(B21,$E$1,100000000)</f>
-        <v>7389.4017502300003</v>
+        <v>7367.3803542899996</v>
       </c>
       <c r="F21" t="str">
         <f>[1]!s_info_thematicindustry_wind(B21,"")</f>
@@ -2456,10 +2495,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FB3FBC3-0643-3F43-8205-9D348FFD3399}">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31:F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2468,6 +2507,7 @@
     <col min="2" max="2" width="15.83203125" customWidth="1"/>
     <col min="3" max="3" width="14.6640625" customWidth="1"/>
     <col min="4" max="4" width="146.5" style="7" customWidth="1"/>
+    <col min="5" max="5" width="43.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -2509,7 +2549,7 @@
         <v>371</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>419</v>
+        <v>434</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -2537,7 +2577,7 @@
         <v>8</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -2551,7 +2591,7 @@
         <v>0</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -2565,7 +2605,7 @@
         <v>6</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -2579,7 +2619,7 @@
         <v>2</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -2592,6 +2632,9 @@
       <c r="C9" t="s">
         <v>367</v>
       </c>
+      <c r="D9" s="8" t="s">
+        <v>425</v>
+      </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
@@ -2603,6 +2646,9 @@
       <c r="C10" t="s">
         <v>368</v>
       </c>
+      <c r="D10" s="8" t="s">
+        <v>426</v>
+      </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
@@ -2614,6 +2660,9 @@
       <c r="C11" t="s">
         <v>369</v>
       </c>
+      <c r="D11" s="8" t="s">
+        <v>427</v>
+      </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
@@ -2625,6 +2674,9 @@
       <c r="C12" t="s">
         <v>372</v>
       </c>
+      <c r="D12" s="7" t="s">
+        <v>432</v>
+      </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
@@ -2637,7 +2689,7 @@
         <v>364</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -2650,6 +2702,9 @@
       <c r="C14" t="s">
         <v>11</v>
       </c>
+      <c r="D14" s="8" t="s">
+        <v>431</v>
+      </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
@@ -2661,6 +2716,9 @@
       <c r="C15" t="s">
         <v>365</v>
       </c>
+      <c r="D15" s="7" t="s">
+        <v>435</v>
+      </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="5" t="s">
@@ -2687,7 +2745,7 @@
         <v>353</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -2700,6 +2758,9 @@
       <c r="C18" t="s">
         <v>14</v>
       </c>
+      <c r="D18" s="7" t="s">
+        <v>433</v>
+      </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
@@ -2711,6 +2772,9 @@
       <c r="C19" t="s">
         <v>4</v>
       </c>
+      <c r="D19" s="8" t="s">
+        <v>429</v>
+      </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
@@ -2722,6 +2786,9 @@
       <c r="C20" t="s">
         <v>13</v>
       </c>
+      <c r="D20" s="8" t="s">
+        <v>428</v>
+      </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
@@ -2733,6 +2800,39 @@
       <c r="C21" t="s">
         <v>370</v>
       </c>
+      <c r="D21" s="8" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="D31" s="4"/>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="D32" s="4"/>
+    </row>
+    <row r="33" spans="4:4">
+      <c r="D33" s="4"/>
+    </row>
+    <row r="34" spans="4:4">
+      <c r="D34" s="4"/>
+    </row>
+    <row r="35" spans="4:4">
+      <c r="D35" s="4"/>
+    </row>
+    <row r="36" spans="4:4">
+      <c r="D36" s="4"/>
+    </row>
+    <row r="37" spans="4:4">
+      <c r="D37" s="4"/>
+    </row>
+    <row r="38" spans="4:4">
+      <c r="D38" s="4"/>
+    </row>
+    <row r="39" spans="4:4">
+      <c r="D39" s="4"/>
+    </row>
+    <row r="40" spans="4:4">
+      <c r="D40" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
Add new method to portfolio optimization
</commit_message>
<xml_diff>
--- a/Stocks.xlsx
+++ b/Stocks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaelxu/My_Document/Michael/金融/量化/Arbitrage/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{512F832F-CC64-5F4D-8E5A-A1B6B1730D17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B96F6E1E-B49A-054D-9A20-7480C6FB0EA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40" yWindow="500" windowWidth="18860" windowHeight="17720" activeTab="1" xr2:uid="{49E41F07-E01F-DB49-9AD6-EC869743E72B}"/>
+    <workbookView xWindow="40" yWindow="500" windowWidth="18860" windowHeight="17720" activeTab="2" xr2:uid="{49E41F07-E01F-DB49-9AD6-EC869743E72B}"/>
   </bookViews>
   <sheets>
     <sheet name="Watchlist" sheetId="1" r:id="rId1"/>
@@ -1874,7 +1874,7 @@
   <dimension ref="A1:I34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1904,7 +1904,7 @@
       </c>
       <c r="E1" s="1">
         <f ca="1">TODAY()</f>
-        <v>45503</v>
+        <v>45511</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>341</v>
@@ -1930,7 +1930,7 @@
       </c>
       <c r="D2" s="2">
         <f ca="1">[1]!s_val_mv_ref(B2,$E$1,100000000)</f>
-        <v>163.63147882000001</v>
+        <v>163.13411869999999</v>
       </c>
       <c r="F2" t="str">
         <f>[1]!s_info_thematicindustry_wind(B2,"")</f>
@@ -1951,7 +1951,7 @@
       </c>
       <c r="D3" s="2">
         <f ca="1">[1]!s_val_mv_ref(B3,$E$1,100000000)</f>
-        <v>13351.990650309999</v>
+        <v>13071.604405800001</v>
       </c>
       <c r="F3" t="str">
         <f>[1]!s_info_thematicindustry_wind(B3,"")</f>
@@ -1972,7 +1972,7 @@
       </c>
       <c r="D4" s="2">
         <f ca="1">[1]!s_val_mv_ref(B4,$E$1,100000000)</f>
-        <v>2223.0635000000002</v>
+        <v>2230.8195000000001</v>
       </c>
       <c r="F4" t="str">
         <f>[1]!s_info_thematicindustry_wind(B4,"")</f>
@@ -1999,7 +1999,7 @@
       </c>
       <c r="D5" s="2">
         <f ca="1">[1]!s_val_mv_ref(B5,$E$1,100000000)</f>
-        <v>1535.35322172</v>
+        <v>1630.8155982000001</v>
       </c>
       <c r="F5" t="str">
         <f>[1]!s_info_thematicindustry_wind(B5,"")</f>
@@ -2026,7 +2026,7 @@
       </c>
       <c r="D6" s="2">
         <f ca="1">[1]!s_val_mv_ref(B6,$E$1,100000000)</f>
-        <v>1546.5056257399999</v>
+        <v>1531.3861573300001</v>
       </c>
       <c r="F6" t="str">
         <f>[1]!s_info_thematicindustry_wind(B6,"")</f>
@@ -2053,7 +2053,7 @@
       </c>
       <c r="D7" s="2">
         <f ca="1">[1]!s_val_mv_ref(B7,$E$1,100000000)</f>
-        <v>619.98379190000003</v>
+        <v>622.15283140999998</v>
       </c>
       <c r="F7" t="str">
         <f>[1]!s_info_thematicindustry_wind(B7,"")</f>
@@ -2083,7 +2083,7 @@
       </c>
       <c r="D8" s="2">
         <f ca="1">[1]!s_val_mv_ref(B8,$E$1,100000000)</f>
-        <v>243.86854145000001</v>
+        <v>245.03588434</v>
       </c>
       <c r="F8" t="str">
         <f>[1]!s_info_thematicindustry_wind(B8,"")</f>
@@ -2110,7 +2110,7 @@
       </c>
       <c r="D9" s="2">
         <f ca="1">[1]!s_val_mv_ref(B9,$E$1,100000000)</f>
-        <v>537.97864665999998</v>
+        <v>550.68680367000002</v>
       </c>
       <c r="F9" t="str">
         <f>[1]!s_info_thematicindustry_wind(B9,"")</f>
@@ -2131,7 +2131,7 @@
       </c>
       <c r="D10" s="2">
         <f ca="1">[1]!s_val_mv_ref(B10,$E$1,100000000)</f>
-        <v>461.01914266</v>
+        <v>463.80921935999999</v>
       </c>
       <c r="F10" t="str">
         <f>[1]!s_info_thematicindustry_wind(B10,"")</f>
@@ -2152,7 +2152,7 @@
       </c>
       <c r="D11" s="2">
         <f ca="1">[1]!s_val_mv_ref(B11,$E$1,100000000)</f>
-        <v>1134.16899917</v>
+        <v>1101.56807484</v>
       </c>
       <c r="F11" t="str">
         <f>[1]!s_info_thematicindustry_wind(B11,"")</f>
@@ -2173,7 +2173,7 @@
       </c>
       <c r="D12" s="2">
         <f ca="1">[1]!s_val_mv_ref(B12,$E$1,100000000)</f>
-        <v>378.30875965000001</v>
+        <v>383.73984099</v>
       </c>
       <c r="F12" t="str">
         <f>[1]!s_info_thematicindustry_wind(B12,"")</f>
@@ -2194,7 +2194,7 @@
       </c>
       <c r="D13" s="2">
         <f ca="1">[1]!s_val_mv_ref(B13,$E$1,100000000)</f>
-        <v>2058.9181694899999</v>
+        <v>2054.1395314400002</v>
       </c>
       <c r="F13" t="str">
         <f>[1]!s_info_thematicindustry_wind(B13,"")</f>
@@ -2215,7 +2215,7 @@
       </c>
       <c r="D14" s="2">
         <f ca="1">[1]!s_val_mv_ref(B14,$E$1,100000000)</f>
-        <v>703.21244062000005</v>
+        <v>706.07490645999997</v>
       </c>
       <c r="F14" t="str">
         <f>[1]!s_info_thematicindustry_wind(B14,"")</f>
@@ -2242,7 +2242,7 @@
       </c>
       <c r="D15" s="2">
         <f ca="1">[1]!s_val_mv_ref(B15,$E$1,100000000)</f>
-        <v>474.81950732000001</v>
+        <v>480.09527961999999</v>
       </c>
       <c r="F15" t="str">
         <f>[1]!s_info_thematicindustry_wind(B15,"")</f>
@@ -2263,7 +2263,7 @@
       </c>
       <c r="D16" s="2">
         <f ca="1">[1]!s_val_mv_ref(B16,$E$1,100000000)</f>
-        <v>199.29814479000001</v>
+        <v>192.20611188999999</v>
       </c>
       <c r="F16" t="str">
         <f>[1]!s_info_thematicindustry_wind(B16,"")</f>
@@ -2290,7 +2290,7 @@
       </c>
       <c r="D17" s="2">
         <f ca="1">[1]!s_val_mv_ref(B17,$E$1,100000000)</f>
-        <v>111.07884931</v>
+        <v>100.45171567</v>
       </c>
       <c r="F17" t="str">
         <f>[1]!s_info_thematicindustry_wind(B17,"")</f>
@@ -2320,7 +2320,7 @@
       </c>
       <c r="D18" s="2">
         <f ca="1">[1]!s_val_mv_ref(B18,$E$1,100000000)</f>
-        <v>601.72496999999998</v>
+        <v>571.86590999999999</v>
       </c>
       <c r="F18" t="str">
         <f>[1]!s_info_thematicindustry_wind(B18,"")</f>
@@ -2347,7 +2347,7 @@
       </c>
       <c r="D19" s="2">
         <f ca="1">[1]!s_val_mv_ref(B19,$E$1,100000000)</f>
-        <v>301.37498642999998</v>
+        <v>283.71992555999998</v>
       </c>
       <c r="F19" t="str">
         <f>[1]!s_info_thematicindustry_wind(B19,"")</f>
@@ -2374,7 +2374,7 @@
       </c>
       <c r="D20" s="2">
         <f ca="1">[1]!s_val_mv_ref(B20,$E$1,100000000)</f>
-        <v>2192.3493730599998</v>
+        <v>2073.3846784000002</v>
       </c>
       <c r="F20" t="str">
         <f>[1]!s_info_thematicindustry_wind(B20,"")</f>
@@ -2401,7 +2401,7 @@
       </c>
       <c r="D21" s="2">
         <f ca="1">[1]!s_val_mv_ref(B21,$E$1,100000000)</f>
-        <v>7367.3803542899996</v>
+        <v>7279.2947705099996</v>
       </c>
       <c r="F21" t="str">
         <f>[1]!s_info_thematicindustry_wind(B21,"")</f>
@@ -2497,7 +2497,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FB3FBC3-0643-3F43-8205-9D348FFD3399}">
   <dimension ref="A1:D40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+    <sheetView topLeftCell="A12" workbookViewId="0">
       <selection activeCell="E31" sqref="E31:F31"/>
     </sheetView>
   </sheetViews>
@@ -2845,7 +2845,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{517AB5AB-9620-794C-95EA-67FCC0B03FDF}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
@@ -3681,7 +3681,7 @@
       </c>
       <c r="E38" t="str">
         <f>[1]!s_info_thematicindustry_wind(A38,"")</f>
-        <v>农业</v>
+        <v>房地产</v>
       </c>
     </row>
     <row r="39" spans="1:5">

</xml_diff>

<commit_message>
update the display table method
</commit_message>
<xml_diff>
--- a/Stocks.xlsx
+++ b/Stocks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaelxu/My_Document/Michael/金融/量化/Arbitrage/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94EC8255-880F-A444-AFBE-4E77A462FF00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8D2FE42-4A20-5F41-9E1D-069CFBB2F763}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2160" yWindow="500" windowWidth="18860" windowHeight="17720" activeTab="3" xr2:uid="{49E41F07-E01F-DB49-9AD6-EC869743E72B}"/>
   </bookViews>
@@ -3603,7 +3603,7 @@
       </c>
       <c r="E1" s="1">
         <f ca="1">TODAY()</f>
-        <v>45516</v>
+        <v>45523</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>341</v>
@@ -3629,7 +3629,7 @@
       </c>
       <c r="D2" s="2">
         <f ca="1">[1]!s_val_mv_ref(B2,$E$1,100000000)</f>
-        <v>163.13411869999999</v>
+        <v>155.42503687999999</v>
       </c>
       <c r="F2" t="str">
         <f>[1]!s_info_thematicindustry_wind(B2,"")</f>
@@ -3650,7 +3650,7 @@
       </c>
       <c r="D3" s="2">
         <f ca="1">[1]!s_val_mv_ref(B3,$E$1,100000000)</f>
-        <v>13390.192072289999</v>
+        <v>13789.61541536</v>
       </c>
       <c r="F3" t="str">
         <f>[1]!s_info_thematicindustry_wind(B3,"")</f>
@@ -3671,7 +3671,7 @@
       </c>
       <c r="D4" s="2">
         <f ca="1">[1]!s_val_mv_ref(B4,$E$1,100000000)</f>
-        <v>2238.5754999999999</v>
+        <v>2355.8850000000002</v>
       </c>
       <c r="F4" t="str">
         <f>[1]!s_info_thematicindustry_wind(B4,"")</f>
@@ -3698,7 +3698,7 @@
       </c>
       <c r="D5" s="2">
         <f ca="1">[1]!s_val_mv_ref(B5,$E$1,100000000)</f>
-        <v>1711.6934449400001</v>
+        <v>1792.5712916800001</v>
       </c>
       <c r="F5" t="str">
         <f>[1]!s_info_thematicindustry_wind(B5,"")</f>
@@ -3725,7 +3725,7 @@
       </c>
       <c r="D6" s="2">
         <f ca="1">[1]!s_val_mv_ref(B6,$E$1,100000000)</f>
-        <v>1537.8659295099999</v>
+        <v>1622.10296778</v>
       </c>
       <c r="F6" t="str">
         <f>[1]!s_info_thematicindustry_wind(B6,"")</f>
@@ -3752,7 +3752,7 @@
       </c>
       <c r="D7" s="2">
         <f ca="1">[1]!s_val_mv_ref(B7,$E$1,100000000)</f>
-        <v>608.05407462000005</v>
+        <v>612.75366022000003</v>
       </c>
       <c r="F7" t="str">
         <f>[1]!s_info_thematicindustry_wind(B7,"")</f>
@@ -3782,7 +3782,7 @@
       </c>
       <c r="D8" s="2">
         <f ca="1">[1]!s_val_mv_ref(B8,$E$1,100000000)</f>
-        <v>237.07672828</v>
+        <v>237.92570492999999</v>
       </c>
       <c r="F8" t="str">
         <f>[1]!s_info_thematicindustry_wind(B8,"")</f>
@@ -3809,7 +3809,7 @@
       </c>
       <c r="D9" s="2">
         <f ca="1">[1]!s_val_mv_ref(B9,$E$1,100000000)</f>
-        <v>536.97006277000003</v>
+        <v>535.35632854999994</v>
       </c>
       <c r="F9" t="str">
         <f>[1]!s_info_thematicindustry_wind(B9,"")</f>
@@ -3830,7 +3830,7 @@
       </c>
       <c r="D10" s="2">
         <f ca="1">[1]!s_val_mv_ref(B10,$E$1,100000000)</f>
-        <v>444.77104899</v>
+        <v>431.96952064999999</v>
       </c>
       <c r="F10" t="str">
         <f>[1]!s_info_thematicindustry_wind(B10,"")</f>
@@ -3851,7 +3851,7 @@
       </c>
       <c r="D11" s="2">
         <f ca="1">[1]!s_val_mv_ref(B11,$E$1,100000000)</f>
-        <v>1125.5898085599999</v>
+        <v>1168.4857616300001</v>
       </c>
       <c r="F11" t="str">
         <f>[1]!s_info_thematicindustry_wind(B11,"")</f>
@@ -3872,7 +3872,7 @@
       </c>
       <c r="D12" s="2">
         <f ca="1">[1]!s_val_mv_ref(B12,$E$1,100000000)</f>
-        <v>377.79959577</v>
+        <v>377.62987448000001</v>
       </c>
       <c r="F12" t="str">
         <f>[1]!s_info_thematicindustry_wind(B12,"")</f>
@@ -3893,7 +3893,7 @@
       </c>
       <c r="D13" s="2">
         <f ca="1">[1]!s_val_mv_ref(B13,$E$1,100000000)</f>
-        <v>1974.3361308399999</v>
+        <v>2027.0063752399999</v>
       </c>
       <c r="F13" t="str">
         <f>[1]!s_info_thematicindustry_wind(B13,"")</f>
@@ -3914,7 +3914,7 @@
       </c>
       <c r="D14" s="2">
         <f ca="1">[1]!s_val_mv_ref(B14,$E$1,100000000)</f>
-        <v>705.59782882000002</v>
+        <v>725.15801204000002</v>
       </c>
       <c r="F14" t="str">
         <f>[1]!s_info_thematicindustry_wind(B14,"")</f>
@@ -3941,7 +3941,7 @@
       </c>
       <c r="D15" s="2">
         <f ca="1">[1]!s_val_mv_ref(B15,$E$1,100000000)</f>
-        <v>480.65062406999999</v>
+        <v>487.03708527999999</v>
       </c>
       <c r="F15" t="str">
         <f>[1]!s_info_thematicindustry_wind(B15,"")</f>
@@ -3962,7 +3962,7 @@
       </c>
       <c r="D16" s="2">
         <f ca="1">[1]!s_val_mv_ref(B16,$E$1,100000000)</f>
-        <v>187.397954</v>
+        <v>196.89406584</v>
       </c>
       <c r="F16" t="str">
         <f>[1]!s_info_thematicindustry_wind(B16,"")</f>
@@ -3989,7 +3989,7 @@
       </c>
       <c r="D17" s="2">
         <f ca="1">[1]!s_val_mv_ref(B17,$E$1,100000000)</f>
-        <v>102.03313436000001</v>
+        <v>101.46382362999999</v>
       </c>
       <c r="F17" t="str">
         <f>[1]!s_info_thematicindustry_wind(B17,"")</f>
@@ -4019,7 +4019,7 @@
       </c>
       <c r="D18" s="2">
         <f ca="1">[1]!s_val_mv_ref(B18,$E$1,100000000)</f>
-        <v>584.19899999999996</v>
+        <v>616.65449999999998</v>
       </c>
       <c r="F18" t="str">
         <f>[1]!s_info_thematicindustry_wind(B18,"")</f>
@@ -4046,7 +4046,7 @@
       </c>
       <c r="D19" s="2">
         <f ca="1">[1]!s_val_mv_ref(B19,$E$1,100000000)</f>
-        <v>2020.5114807699999</v>
+        <v>2133.8111899700002</v>
       </c>
       <c r="F19" t="str">
         <f>[1]!s_info_thematicindustry_wind(B19,"")</f>
@@ -4073,7 +4073,7 @@
       </c>
       <c r="D20" s="2">
         <f ca="1">[1]!s_val_mv_ref(B20,$E$1,100000000)</f>
-        <v>7139.8259295300004</v>
+        <v>7274.4011269700004</v>
       </c>
       <c r="F20" t="str">
         <f>[1]!s_info_thematicindustry_wind(B20,"")</f>
@@ -9184,7 +9184,7 @@
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -9318,171 +9318,171 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>366</v>
+        <v>371</v>
       </c>
       <c r="B10" t="str">
         <f t="shared" si="0"/>
-        <v>002299.SZ</v>
+        <v>600938.SH</v>
       </c>
       <c r="C10" t="str">
         <f>[1]!s_info_name(B10)</f>
-        <v>圣农发展</v>
+        <v>中国海油</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>371</v>
+        <v>9</v>
       </c>
       <c r="B11" t="str">
         <f t="shared" si="0"/>
-        <v>600938.SH</v>
+        <v>601225.SH</v>
       </c>
       <c r="C11" t="str">
         <f>[1]!s_info_name(B11)</f>
-        <v>中国海油</v>
+        <v>陕西煤业</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B12" t="str">
         <f t="shared" si="0"/>
-        <v>601225.SH</v>
+        <v>601898.SH</v>
       </c>
       <c r="C12" t="str">
         <f>[1]!s_info_name(B12)</f>
-        <v>陕西煤业</v>
+        <v>中煤能源</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="B13" t="str">
         <f t="shared" si="0"/>
-        <v>601898.SH</v>
+        <v>603993.SH</v>
       </c>
       <c r="C13" t="str">
         <f>[1]!s_info_name(B13)</f>
-        <v>中煤能源</v>
+        <v>洛阳钼业</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>0</v>
+        <v>364</v>
       </c>
       <c r="B14" t="str">
         <f t="shared" si="0"/>
-        <v>603993.SH</v>
+        <v>601919.SH</v>
       </c>
       <c r="C14" t="str">
         <f>[1]!s_info_name(B14)</f>
-        <v>洛阳钼业</v>
+        <v>中远海控</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>364</v>
+        <v>11</v>
       </c>
       <c r="B15" t="str">
         <f t="shared" si="0"/>
-        <v>601919.SH</v>
+        <v>600026.SH</v>
       </c>
       <c r="C15" t="str">
         <f>[1]!s_info_name(B15)</f>
-        <v>中远海控</v>
+        <v>中远海能</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>11</v>
+        <v>365</v>
       </c>
       <c r="B16" t="str">
         <f t="shared" si="0"/>
-        <v>600026.SH</v>
+        <v>000975.SZ</v>
       </c>
       <c r="C16" t="str">
         <f>[1]!s_info_name(B16)</f>
-        <v>中远海能</v>
+        <v>山金国际</v>
       </c>
     </row>
     <row r="17" spans="1:3">
-      <c r="A17" t="s">
-        <v>365</v>
-      </c>
-      <c r="B17" t="str">
+      <c r="A17" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B17" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>000975.SZ</v>
-      </c>
-      <c r="C17" t="str">
+        <v>002155.SZ</v>
+      </c>
+      <c r="C17" s="5" t="str">
         <f>[1]!s_info_name(B17)</f>
-        <v>山金国际</v>
+        <v>湖南黄金</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="5" t="s">
-        <v>3</v>
+        <v>353</v>
       </c>
       <c r="B18" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>002155.SZ</v>
+        <v>600301.SH</v>
       </c>
       <c r="C18" s="5" t="str">
         <f>[1]!s_info_name(B18)</f>
-        <v>湖南黄金</v>
+        <v>华锡有色</v>
       </c>
     </row>
     <row r="19" spans="1:3">
-      <c r="A19" s="5" t="s">
-        <v>353</v>
-      </c>
-      <c r="B19" s="5" t="str">
+      <c r="A19" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" t="str">
         <f t="shared" si="0"/>
-        <v>600301.SH</v>
-      </c>
-      <c r="C19" s="5" t="str">
+        <v>601298.SH</v>
+      </c>
+      <c r="C19" t="str">
         <f>[1]!s_info_name(B19)</f>
-        <v>华锡有色</v>
+        <v>青岛港</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B20" t="str">
         <f t="shared" si="0"/>
-        <v>601298.SH</v>
+        <v>601985.SH</v>
       </c>
       <c r="C20" t="str">
         <f>[1]!s_info_name(B20)</f>
-        <v>青岛港</v>
+        <v>中国核电</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" t="s">
-        <v>13</v>
+        <v>370</v>
       </c>
       <c r="B21" t="str">
         <f t="shared" si="0"/>
-        <v>601985.SH</v>
+        <v>600900.SH</v>
       </c>
       <c r="C21" t="str">
         <f>[1]!s_info_name(B21)</f>
-        <v>中国核电</v>
+        <v>长江电力</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
       <c r="B22" t="str">
         <f t="shared" si="0"/>
-        <v>600900.SH</v>
+        <v>002299.SZ</v>
       </c>
       <c r="C22" t="str">
         <f>[1]!s_info_name(B22)</f>
-        <v>长江电力</v>
+        <v>圣农发展</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
transfer the function to portfolio_utils.py
</commit_message>
<xml_diff>
--- a/Stocks.xlsx
+++ b/Stocks.xlsx
@@ -8,20 +8,24 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaelxu/My_Document/Michael/金融/量化/Arbitrage/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8D2FE42-4A20-5F41-9E1D-069CFBB2F763}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F85161B9-6F5D-0941-B48A-BF8C469C6F82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2160" yWindow="500" windowWidth="18860" windowHeight="17720" activeTab="3" xr2:uid="{49E41F07-E01F-DB49-9AD6-EC869743E72B}"/>
+    <workbookView xWindow="12140" yWindow="500" windowWidth="17460" windowHeight="17720" activeTab="4" xr2:uid="{49E41F07-E01F-DB49-9AD6-EC869743E72B}"/>
   </bookViews>
   <sheets>
     <sheet name="Watchlist" sheetId="1" r:id="rId1"/>
     <sheet name="HS300" sheetId="9" r:id="rId2"/>
     <sheet name="Target-Pair" sheetId="8" r:id="rId3"/>
     <sheet name="Holdlist" sheetId="7" r:id="rId4"/>
-    <sheet name="Test" sheetId="6" r:id="rId5"/>
+    <sheet name="ETF" sheetId="10" r:id="rId5"/>
+    <sheet name="Test" sheetId="6" r:id="rId6"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId6"/>
+    <externalReference r:id="rId7"/>
   </externalReferences>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">ETF!$A$1:$A$6</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -43,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1676" uniqueCount="1000">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1690" uniqueCount="1006">
   <si>
     <t>603993.SS</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -3113,6 +3117,30 @@
   </si>
   <si>
     <t>000001.SZ</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Target</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>^NDXX</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>^NDX</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>^SPX</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GC=F</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>^IXIC</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -3603,7 +3631,7 @@
       </c>
       <c r="E1" s="1">
         <f ca="1">TODAY()</f>
-        <v>45523</v>
+        <v>45527</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>341</v>
@@ -3629,7 +3657,7 @@
       </c>
       <c r="D2" s="2">
         <f ca="1">[1]!s_val_mv_ref(B2,$E$1,100000000)</f>
-        <v>155.42503687999999</v>
+        <v>148.83501530999999</v>
       </c>
       <c r="F2" t="str">
         <f>[1]!s_info_thematicindustry_wind(B2,"")</f>
@@ -3650,7 +3678,7 @@
       </c>
       <c r="D3" s="2">
         <f ca="1">[1]!s_val_mv_ref(B3,$E$1,100000000)</f>
-        <v>13789.61541536</v>
+        <v>13280.826156929999</v>
       </c>
       <c r="F3" t="str">
         <f>[1]!s_info_thematicindustry_wind(B3,"")</f>
@@ -3671,7 +3699,7 @@
       </c>
       <c r="D4" s="2">
         <f ca="1">[1]!s_val_mv_ref(B4,$E$1,100000000)</f>
-        <v>2355.8850000000002</v>
+        <v>2292.8674999999998</v>
       </c>
       <c r="F4" t="str">
         <f>[1]!s_info_thematicindustry_wind(B4,"")</f>
@@ -3698,7 +3726,7 @@
       </c>
       <c r="D5" s="2">
         <f ca="1">[1]!s_val_mv_ref(B5,$E$1,100000000)</f>
-        <v>1792.5712916800001</v>
+        <v>1718.32277664</v>
       </c>
       <c r="F5" t="str">
         <f>[1]!s_info_thematicindustry_wind(B5,"")</f>
@@ -3725,7 +3753,7 @@
       </c>
       <c r="D6" s="2">
         <f ca="1">[1]!s_val_mv_ref(B6,$E$1,100000000)</f>
-        <v>1622.10296778</v>
+        <v>1602.6636512600001</v>
       </c>
       <c r="F6" t="str">
         <f>[1]!s_info_thematicindustry_wind(B6,"")</f>
@@ -3752,7 +3780,7 @@
       </c>
       <c r="D7" s="2">
         <f ca="1">[1]!s_val_mv_ref(B7,$E$1,100000000)</f>
-        <v>612.75366022000003</v>
+        <v>588.53271907999999</v>
       </c>
       <c r="F7" t="str">
         <f>[1]!s_info_thematicindustry_wind(B7,"")</f>
@@ -3782,7 +3810,7 @@
       </c>
       <c r="D8" s="2">
         <f ca="1">[1]!s_val_mv_ref(B8,$E$1,100000000)</f>
-        <v>237.92570492999999</v>
+        <v>226.46452020999999</v>
       </c>
       <c r="F8" t="str">
         <f>[1]!s_info_thematicindustry_wind(B8,"")</f>
@@ -3809,7 +3837,7 @@
       </c>
       <c r="D9" s="2">
         <f ca="1">[1]!s_val_mv_ref(B9,$E$1,100000000)</f>
-        <v>535.35632854999994</v>
+        <v>514.78121720000001</v>
       </c>
       <c r="F9" t="str">
         <f>[1]!s_info_thematicindustry_wind(B9,"")</f>
@@ -3830,7 +3858,7 @@
       </c>
       <c r="D10" s="2">
         <f ca="1">[1]!s_val_mv_ref(B10,$E$1,100000000)</f>
-        <v>431.96952064999999</v>
+        <v>412.11073949000001</v>
       </c>
       <c r="F10" t="str">
         <f>[1]!s_info_thematicindustry_wind(B10,"")</f>
@@ -3851,7 +3879,7 @@
       </c>
       <c r="D11" s="2">
         <f ca="1">[1]!s_val_mv_ref(B11,$E$1,100000000)</f>
-        <v>1168.4857616300001</v>
+        <v>1163.3382472599999</v>
       </c>
       <c r="F11" t="str">
         <f>[1]!s_info_thematicindustry_wind(B11,"")</f>
@@ -3872,7 +3900,7 @@
       </c>
       <c r="D12" s="2">
         <f ca="1">[1]!s_val_mv_ref(B12,$E$1,100000000)</f>
-        <v>377.62987448000001</v>
+        <v>365.07049888</v>
       </c>
       <c r="F12" t="str">
         <f>[1]!s_info_thematicindustry_wind(B12,"")</f>
@@ -3893,7 +3921,7 @@
       </c>
       <c r="D13" s="2">
         <f ca="1">[1]!s_val_mv_ref(B13,$E$1,100000000)</f>
-        <v>2027.0063752399999</v>
+        <v>1974.3361308399999</v>
       </c>
       <c r="F13" t="str">
         <f>[1]!s_info_thematicindustry_wind(B13,"")</f>
@@ -3914,7 +3942,7 @@
       </c>
       <c r="D14" s="2">
         <f ca="1">[1]!s_val_mv_ref(B14,$E$1,100000000)</f>
-        <v>725.15801204000002</v>
+        <v>700.82705242999998</v>
       </c>
       <c r="F14" t="str">
         <f>[1]!s_info_thematicindustry_wind(B14,"")</f>
@@ -3962,7 +3990,7 @@
       </c>
       <c r="D16" s="2">
         <f ca="1">[1]!s_val_mv_ref(B16,$E$1,100000000)</f>
-        <v>196.89406584</v>
+        <v>191.00407242</v>
       </c>
       <c r="F16" t="str">
         <f>[1]!s_info_thematicindustry_wind(B16,"")</f>
@@ -3989,7 +4017,7 @@
       </c>
       <c r="D17" s="2">
         <f ca="1">[1]!s_val_mv_ref(B17,$E$1,100000000)</f>
-        <v>101.46382362999999</v>
+        <v>101.14753989</v>
       </c>
       <c r="F17" t="str">
         <f>[1]!s_info_thematicindustry_wind(B17,"")</f>
@@ -4019,7 +4047,7 @@
       </c>
       <c r="D18" s="2">
         <f ca="1">[1]!s_val_mv_ref(B18,$E$1,100000000)</f>
-        <v>616.65449999999998</v>
+        <v>614.70717000000002</v>
       </c>
       <c r="F18" t="str">
         <f>[1]!s_info_thematicindustry_wind(B18,"")</f>
@@ -4046,7 +4074,7 @@
       </c>
       <c r="D19" s="2">
         <f ca="1">[1]!s_val_mv_ref(B19,$E$1,100000000)</f>
-        <v>2133.8111899700002</v>
+        <v>2135.69951846</v>
       </c>
       <c r="F19" t="str">
         <f>[1]!s_info_thematicindustry_wind(B19,"")</f>
@@ -4073,7 +4101,7 @@
       </c>
       <c r="D20" s="2">
         <f ca="1">[1]!s_val_mv_ref(B20,$E$1,100000000)</f>
-        <v>7274.4011269700004</v>
+        <v>7318.4439188599999</v>
       </c>
       <c r="F20" t="str">
         <f>[1]!s_info_thematicindustry_wind(B20,"")</f>
@@ -9183,8 +9211,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{517AB5AB-9620-794C-95EA-67FCC0B03FDF}">
   <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -9493,6 +9521,127 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22D975BE-60A2-DA49-B9A5-6A73F6FBEA18}">
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="14" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" customWidth="1"/>
+    <col min="3" max="3" width="16.6640625" customWidth="1"/>
+    <col min="4" max="4" width="18.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>355</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="5" t="s">
+        <v>362</v>
+      </c>
+      <c r="B2" s="5" t="str">
+        <f t="shared" ref="B2:B6" si="0">SUBSTITUTE(A2,"SS","SH")</f>
+        <v>159509.SZ</v>
+      </c>
+      <c r="C2" s="5" t="str">
+        <f>[1]!s_info_name(B2)</f>
+        <v>纳指科技ETF</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="5" t="s">
+        <v>360</v>
+      </c>
+      <c r="B3" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>513110.SH</v>
+      </c>
+      <c r="C3" s="5" t="str">
+        <f>[1]!s_info_name(B3)</f>
+        <v>纳斯达克100ETF</v>
+      </c>
+      <c r="D3" t="s">
+        <v>1002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="5" t="s">
+        <v>357</v>
+      </c>
+      <c r="B4" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>513300.SH</v>
+      </c>
+      <c r="C4" s="5" t="str">
+        <f>[1]!s_info_name(B4)</f>
+        <v>纳斯达克ETF</v>
+      </c>
+      <c r="D4" t="s">
+        <v>1005</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="5" t="s">
+        <v>356</v>
+      </c>
+      <c r="B5" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>513500.SH</v>
+      </c>
+      <c r="C5" s="5" t="str">
+        <f>[1]!s_info_name(B5)</f>
+        <v>标普500ETF</v>
+      </c>
+      <c r="D5" t="s">
+        <v>1003</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>518880.SH</v>
+      </c>
+      <c r="C6" s="5" t="str">
+        <f>[1]!s_info_name(B6)</f>
+        <v>黄金ETF</v>
+      </c>
+      <c r="D6" t="s">
+        <v>1004</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:A6" xr:uid="{22D975BE-60A2-DA49-B9A5-6A73F6FBEA18}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C6">
+      <sortCondition ref="A1:A6"/>
+    </sortState>
+  </autoFilter>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E9EFCA7-AA89-6B4C-9A82-4698CA99580D}">
   <dimension ref="A1:E151"/>
   <sheetViews>

</xml_diff>

<commit_message>
update to aug 30
</commit_message>
<xml_diff>
--- a/Stocks.xlsx
+++ b/Stocks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaelxu/My_Document/Michael/金融/量化/Arbitrage/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F85161B9-6F5D-0941-B48A-BF8C469C6F82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7749905B-251B-E449-9D82-C7DB92DFA380}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12140" yWindow="500" windowWidth="17460" windowHeight="17720" activeTab="4" xr2:uid="{49E41F07-E01F-DB49-9AD6-EC869743E72B}"/>
+    <workbookView xWindow="12140" yWindow="500" windowWidth="17460" windowHeight="17720" activeTab="3" xr2:uid="{49E41F07-E01F-DB49-9AD6-EC869743E72B}"/>
   </bookViews>
   <sheets>
     <sheet name="Watchlist" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1690" uniqueCount="1006">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1684" uniqueCount="1006">
   <si>
     <t>603993.SS</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -3631,7 +3631,7 @@
       </c>
       <c r="E1" s="1">
         <f ca="1">TODAY()</f>
-        <v>45527</v>
+        <v>45533</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>341</v>
@@ -3657,7 +3657,7 @@
       </c>
       <c r="D2" s="2">
         <f ca="1">[1]!s_val_mv_ref(B2,$E$1,100000000)</f>
-        <v>148.83501530999999</v>
+        <v>149.70539552</v>
       </c>
       <c r="F2" t="str">
         <f>[1]!s_info_thematicindustry_wind(B2,"")</f>
@@ -3678,7 +3678,7 @@
       </c>
       <c r="D3" s="2">
         <f ca="1">[1]!s_val_mv_ref(B3,$E$1,100000000)</f>
-        <v>13280.826156929999</v>
+        <v>13789.61541536</v>
       </c>
       <c r="F3" t="str">
         <f>[1]!s_info_thematicindustry_wind(B3,"")</f>
@@ -3699,7 +3699,7 @@
       </c>
       <c r="D4" s="2">
         <f ca="1">[1]!s_val_mv_ref(B4,$E$1,100000000)</f>
-        <v>2292.8674999999998</v>
+        <v>2317.105</v>
       </c>
       <c r="F4" t="str">
         <f>[1]!s_info_thematicindustry_wind(B4,"")</f>
@@ -3726,7 +3726,7 @@
       </c>
       <c r="D5" s="2">
         <f ca="1">[1]!s_val_mv_ref(B5,$E$1,100000000)</f>
-        <v>1718.32277664</v>
+        <v>1789.9195589999999</v>
       </c>
       <c r="F5" t="str">
         <f>[1]!s_info_thematicindustry_wind(B5,"")</f>
@@ -3780,7 +3780,7 @@
       </c>
       <c r="D7" s="2">
         <f ca="1">[1]!s_val_mv_ref(B7,$E$1,100000000)</f>
-        <v>588.53271907999999</v>
+        <v>602.63147586000002</v>
       </c>
       <c r="F7" t="str">
         <f>[1]!s_info_thematicindustry_wind(B7,"")</f>
@@ -3810,7 +3810,7 @@
       </c>
       <c r="D8" s="2">
         <f ca="1">[1]!s_val_mv_ref(B8,$E$1,100000000)</f>
-        <v>226.46452020999999</v>
+        <v>233.89306586000001</v>
       </c>
       <c r="F8" t="str">
         <f>[1]!s_info_thematicindustry_wind(B8,"")</f>
@@ -3837,7 +3837,7 @@
       </c>
       <c r="D9" s="2">
         <f ca="1">[1]!s_val_mv_ref(B9,$E$1,100000000)</f>
-        <v>514.78121720000001</v>
+        <v>532.33057687999997</v>
       </c>
       <c r="F9" t="str">
         <f>[1]!s_info_thematicindustry_wind(B9,"")</f>
@@ -3858,7 +3858,7 @@
       </c>
       <c r="D10" s="2">
         <f ca="1">[1]!s_val_mv_ref(B10,$E$1,100000000)</f>
-        <v>412.11073949000001</v>
+        <v>419.66035877000002</v>
       </c>
       <c r="F10" t="str">
         <f>[1]!s_info_thematicindustry_wind(B10,"")</f>
@@ -3879,7 +3879,7 @@
       </c>
       <c r="D11" s="2">
         <f ca="1">[1]!s_val_mv_ref(B11,$E$1,100000000)</f>
-        <v>1163.3382472599999</v>
+        <v>1173.633276</v>
       </c>
       <c r="F11" t="str">
         <f>[1]!s_info_thematicindustry_wind(B11,"")</f>
@@ -3900,7 +3900,7 @@
       </c>
       <c r="D12" s="2">
         <f ca="1">[1]!s_val_mv_ref(B12,$E$1,100000000)</f>
-        <v>365.07049888</v>
+        <v>384.92789003000001</v>
       </c>
       <c r="F12" t="str">
         <f>[1]!s_info_thematicindustry_wind(B12,"")</f>
@@ -3921,7 +3921,7 @@
       </c>
       <c r="D13" s="2">
         <f ca="1">[1]!s_val_mv_ref(B13,$E$1,100000000)</f>
-        <v>1974.3361308399999</v>
+        <v>1939.22263458</v>
       </c>
       <c r="F13" t="str">
         <f>[1]!s_info_thematicindustry_wind(B13,"")</f>
@@ -3942,7 +3942,7 @@
       </c>
       <c r="D14" s="2">
         <f ca="1">[1]!s_val_mv_ref(B14,$E$1,100000000)</f>
-        <v>700.82705242999998</v>
+        <v>699.87289714999997</v>
       </c>
       <c r="F14" t="str">
         <f>[1]!s_info_thematicindustry_wind(B14,"")</f>
@@ -3969,7 +3969,7 @@
       </c>
       <c r="D15" s="2">
         <f ca="1">[1]!s_val_mv_ref(B15,$E$1,100000000)</f>
-        <v>487.03708527999999</v>
+        <v>470.09907945999998</v>
       </c>
       <c r="F15" t="str">
         <f>[1]!s_info_thematicindustry_wind(B15,"")</f>
@@ -3990,7 +3990,7 @@
       </c>
       <c r="D16" s="2">
         <f ca="1">[1]!s_val_mv_ref(B16,$E$1,100000000)</f>
-        <v>191.00407242</v>
+        <v>187.397954</v>
       </c>
       <c r="F16" t="str">
         <f>[1]!s_info_thematicindustry_wind(B16,"")</f>
@@ -4017,7 +4017,7 @@
       </c>
       <c r="D17" s="2">
         <f ca="1">[1]!s_val_mv_ref(B17,$E$1,100000000)</f>
-        <v>101.14753989</v>
+        <v>101.46382362999999</v>
       </c>
       <c r="F17" t="str">
         <f>[1]!s_info_thematicindustry_wind(B17,"")</f>
@@ -4047,7 +4047,7 @@
       </c>
       <c r="D18" s="2">
         <f ca="1">[1]!s_val_mv_ref(B18,$E$1,100000000)</f>
-        <v>614.70717000000002</v>
+        <v>604.32141000000001</v>
       </c>
       <c r="F18" t="str">
         <f>[1]!s_info_thematicindustry_wind(B18,"")</f>
@@ -4074,7 +4074,7 @@
       </c>
       <c r="D19" s="2">
         <f ca="1">[1]!s_val_mv_ref(B19,$E$1,100000000)</f>
-        <v>2135.69951846</v>
+        <v>2079.0496638599998</v>
       </c>
       <c r="F19" t="str">
         <f>[1]!s_info_thematicindustry_wind(B19,"")</f>
@@ -4101,7 +4101,7 @@
       </c>
       <c r="D20" s="2">
         <f ca="1">[1]!s_val_mv_ref(B20,$E$1,100000000)</f>
-        <v>7318.4439188599999</v>
+        <v>7183.8687214199999</v>
       </c>
       <c r="F20" t="str">
         <f>[1]!s_info_thematicindustry_wind(B20,"")</f>
@@ -9209,10 +9209,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{517AB5AB-9620-794C-95EA-67FCC0B03FDF}">
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:C9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -9242,7 +9242,7 @@
         <v>356</v>
       </c>
       <c r="B2" s="5" t="str">
-        <f t="shared" ref="B2:B22" si="0">SUBSTITUTE(A2,"SS","SH")</f>
+        <f t="shared" ref="B2:B16" si="0">SUBSTITUTE(A2,"SS","SH")</f>
         <v>513500.SH</v>
       </c>
       <c r="C2" s="5" t="str">
@@ -9346,170 +9346,92 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>371</v>
+        <v>0</v>
       </c>
       <c r="B10" t="str">
         <f t="shared" si="0"/>
-        <v>600938.SH</v>
+        <v>603993.SH</v>
       </c>
       <c r="C10" t="str">
         <f>[1]!s_info_name(B10)</f>
-        <v>中国海油</v>
+        <v>洛阳钼业</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>364</v>
       </c>
       <c r="B11" t="str">
         <f t="shared" si="0"/>
-        <v>601225.SH</v>
+        <v>601919.SH</v>
       </c>
       <c r="C11" t="str">
         <f>[1]!s_info_name(B11)</f>
-        <v>陕西煤业</v>
+        <v>中远海控</v>
       </c>
     </row>
     <row r="12" spans="1:4">
-      <c r="A12" t="s">
-        <v>8</v>
-      </c>
-      <c r="B12" t="str">
+      <c r="A12" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>601898.SH</v>
-      </c>
-      <c r="C12" t="str">
+        <v>002155.SZ</v>
+      </c>
+      <c r="C12" s="5" t="str">
         <f>[1]!s_info_name(B12)</f>
-        <v>中煤能源</v>
+        <v>湖南黄金</v>
       </c>
     </row>
     <row r="13" spans="1:4">
-      <c r="A13" t="s">
-        <v>0</v>
-      </c>
-      <c r="B13" t="str">
+      <c r="A13" s="5" t="s">
+        <v>353</v>
+      </c>
+      <c r="B13" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>603993.SH</v>
-      </c>
-      <c r="C13" t="str">
+        <v>600301.SH</v>
+      </c>
+      <c r="C13" s="5" t="str">
         <f>[1]!s_info_name(B13)</f>
-        <v>洛阳钼业</v>
+        <v>华锡有色</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>364</v>
+        <v>14</v>
       </c>
       <c r="B14" t="str">
         <f t="shared" si="0"/>
-        <v>601919.SH</v>
+        <v>601298.SH</v>
       </c>
       <c r="C14" t="str">
         <f>[1]!s_info_name(B14)</f>
-        <v>中远海控</v>
+        <v>青岛港</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B15" t="str">
         <f t="shared" si="0"/>
-        <v>600026.SH</v>
+        <v>601985.SH</v>
       </c>
       <c r="C15" t="str">
         <f>[1]!s_info_name(B15)</f>
-        <v>中远海能</v>
+        <v>中国核电</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="B16" t="str">
         <f t="shared" si="0"/>
-        <v>000975.SZ</v>
+        <v>002299.SZ</v>
       </c>
       <c r="C16" t="str">
         <f>[1]!s_info_name(B16)</f>
-        <v>山金国际</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B17" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>002155.SZ</v>
-      </c>
-      <c r="C17" s="5" t="str">
-        <f>[1]!s_info_name(B17)</f>
-        <v>湖南黄金</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18" s="5" t="s">
-        <v>353</v>
-      </c>
-      <c r="B18" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>600301.SH</v>
-      </c>
-      <c r="C18" s="5" t="str">
-        <f>[1]!s_info_name(B18)</f>
-        <v>华锡有色</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" t="s">
-        <v>14</v>
-      </c>
-      <c r="B19" t="str">
-        <f t="shared" si="0"/>
-        <v>601298.SH</v>
-      </c>
-      <c r="C19" t="str">
-        <f>[1]!s_info_name(B19)</f>
-        <v>青岛港</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20" t="s">
-        <v>13</v>
-      </c>
-      <c r="B20" t="str">
-        <f t="shared" si="0"/>
-        <v>601985.SH</v>
-      </c>
-      <c r="C20" t="str">
-        <f>[1]!s_info_name(B20)</f>
-        <v>中国核电</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21" t="s">
-        <v>370</v>
-      </c>
-      <c r="B21" t="str">
-        <f t="shared" si="0"/>
-        <v>600900.SH</v>
-      </c>
-      <c r="C21" t="str">
-        <f>[1]!s_info_name(B21)</f>
-        <v>长江电力</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="A22" t="s">
-        <v>366</v>
-      </c>
-      <c r="B22" t="str">
-        <f t="shared" si="0"/>
-        <v>002299.SZ</v>
-      </c>
-      <c r="C22" t="str">
-        <f>[1]!s_info_name(B22)</f>
         <v>圣农发展</v>
       </c>
     </row>
@@ -9524,7 +9446,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22D975BE-60A2-DA49-B9A5-6A73F6FBEA18}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>

</xml_diff>